<commit_message>
Connection between boxes and Products - Test
</commit_message>
<xml_diff>
--- a/Barcode/products.xlsx
+++ b/Barcode/products.xlsx
@@ -424,13 +424,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" activeCellId="1" sqref="H13 C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="5.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="14.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -589,6 +589,36 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>A4846885A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-06-09 15:07:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>48836138</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-06-09 15:07:33</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>